<commit_message>
Update tracking Aug 7th
</commit_message>
<xml_diff>
--- a/Project_Planning/Work_Progress/Tracking Progress.xlsx
+++ b/Project_Planning/Work_Progress/Tracking Progress.xlsx
@@ -1,21 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46121C3B-46CE-4926-8B9D-F9E68148949E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Track Table" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Track Table" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -76,7 +67,7 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>MOSBius Interface Study</t>
+    <t xml:space="preserve">MOSBius Interface </t>
   </si>
   <si>
     <t>TT in process</t>
@@ -85,15 +76,15 @@
     <t>Ring Oscillator</t>
   </si>
   <si>
+    <t>PVT/MC in process</t>
+  </si>
+  <si>
     <t>XOR Phase Detector</t>
   </si>
   <si>
     <t>P1</t>
   </si>
   <si>
-    <t>Not started</t>
-  </si>
-  <si>
     <t>Comparator</t>
   </si>
   <si>
@@ -106,37 +97,36 @@
     <t>P2</t>
   </si>
   <si>
+    <t>Low Pass Filter</t>
+  </si>
+  <si>
+    <t>Neuron</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Chip Integration</t>
+  </si>
+  <si>
     <t>Blocked</t>
-  </si>
-  <si>
-    <t>Low Pass Filter</t>
-  </si>
-  <si>
-    <t>Neuron</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Chip Integration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="d/M/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -147,17 +137,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="13">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF374139"/>
@@ -171,7 +155,6 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -186,7 +169,6 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -201,7 +183,6 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -216,7 +197,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -231,7 +211,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -246,7 +225,6 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -261,7 +239,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -276,7 +253,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -291,7 +267,6 @@
       <bottom style="thin">
         <color rgb="FFF6F8F9"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -306,7 +281,6 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -321,7 +295,6 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -336,165 +309,175 @@
       <bottom style="thin">
         <color rgb="FF374139"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF49564C"/>
+          <bgColor rgb="FF49564C"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF6F8F9"/>
           <bgColor rgb="FFF6F8F9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF49564C"/>
-          <bgColor rgb="FF49564C"/>
-        </patternFill>
-      </fill>
+      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Track Table-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    <tableStyle count="3" pivot="0" name="Track Table-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Chipathon_2025_Project" displayName="Chipathon_2025_Project" ref="A1:L16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L16" displayName="Chipathon_2025_Project" name="Chipathon_2025_Project" id="1">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Block"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Priority             (P0 &gt; P3)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Propietario"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Estimated End date"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Logro"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Producto final"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Schematic status"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Layout Status"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PEX Status"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Notes"/>
+    <tableColumn name="Block" id="1"/>
+    <tableColumn name="Priority             (P0 &gt; P3)" id="2"/>
+    <tableColumn name="Propietario" id="3"/>
+    <tableColumn name="Status" id="4"/>
+    <tableColumn name="Start Date" id="5"/>
+    <tableColumn name="Estimated End date" id="6"/>
+    <tableColumn name="Logro" id="7"/>
+    <tableColumn name="Producto final" id="8"/>
+    <tableColumn name="Schematic status" id="9"/>
+    <tableColumn name="Layout Status" id="10"/>
+    <tableColumn name="PEX Status" id="11"/>
+    <tableColumn name="Notes" id="12"/>
   </tableColumns>
-  <tableStyleInfo name="Track Table-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Track Table-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -684,38 +667,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1"/>
-    <col min="11" max="12" width="24.28515625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="27.0"/>
+    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col customWidth="1" hidden="1" min="3" max="3" width="15.13"/>
+    <col customWidth="1" min="4" max="4" width="17.88"/>
+    <col customWidth="1" min="5" max="6" width="17.5"/>
+    <col customWidth="1" hidden="1" min="7" max="7" width="20.13"/>
+    <col customWidth="1" hidden="1" min="8" max="8" width="22.63"/>
+    <col customWidth="1" min="9" max="9" width="21.0"/>
+    <col customWidth="1" min="10" max="10" width="26.13"/>
+    <col customWidth="1" min="11" max="12" width="24.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -765,10 +745,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="7">
-        <v>45838</v>
+        <v>45838.0</v>
       </c>
       <c r="F2" s="7">
-        <v>45871</v>
+        <v>45871.0</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -783,7 +763,7 @@
       </c>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -795,10 +775,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="13">
-        <v>45853</v>
+        <v>45853.0</v>
       </c>
       <c r="F3" s="13">
-        <v>45871</v>
+        <v>45871.0</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -813,7 +793,7 @@
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -825,15 +805,15 @@
         <v>14</v>
       </c>
       <c r="E4" s="7">
-        <v>45866</v>
+        <v>45866.0</v>
       </c>
       <c r="F4" s="7">
-        <v>45878</v>
+        <v>45878.0</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>16</v>
@@ -843,27 +823,27 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E5" s="13">
-        <v>45873</v>
+        <v>45867.0</v>
       </c>
       <c r="F5" s="13">
-        <v>45880</v>
+        <v>45880.0</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>17</v>
@@ -873,7 +853,7 @@
       </c>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -882,18 +862,18 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7">
-        <v>45880</v>
+        <v>45867.0</v>
       </c>
       <c r="F6" s="7">
-        <v>45892</v>
+        <v>45892.0</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>17</v>
@@ -903,27 +883,27 @@
       </c>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7" s="13">
-        <v>45887</v>
+        <v>45874.0</v>
       </c>
       <c r="F7" s="13">
-        <v>45892</v>
+        <v>45892.0</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>17</v>
@@ -933,7 +913,7 @@
       </c>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -942,18 +922,18 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E8" s="7">
-        <v>45894</v>
+        <v>45869.0</v>
       </c>
       <c r="F8" s="7">
-        <v>45906</v>
+        <v>45906.0</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>17</v>
@@ -963,27 +943,27 @@
       </c>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="11" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E9" s="13">
-        <v>45908</v>
+        <v>45910.0</v>
       </c>
       <c r="F9" s="13">
-        <v>45913</v>
+        <v>45913.0</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>17</v>
@@ -993,27 +973,27 @@
       </c>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E10" s="7">
-        <v>45908</v>
+        <v>45910.0</v>
       </c>
       <c r="F10" s="7">
-        <v>45915</v>
+        <v>45915.0</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>17</v>
@@ -1023,22 +1003,22 @@
       </c>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E11" s="13">
-        <v>45915</v>
+        <v>45915.0</v>
       </c>
       <c r="F11" s="13">
-        <v>45926</v>
+        <v>45926.0</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1053,7 +1033,7 @@
       </c>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="8"/>
@@ -1069,7 +1049,7 @@
       <c r="K12" s="17"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="14"/>
@@ -1085,7 +1065,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="16"/>
       <c r="B14" s="17"/>
       <c r="C14" s="8"/>
@@ -1101,7 +1081,7 @@
       <c r="K14" s="17"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="14"/>
@@ -1117,7 +1097,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
@@ -1134,30 +1114,30 @@
       <c r="L16" s="27"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D16">
       <formula1>"Not started,In progress,Blocked,Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I16" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I16">
       <formula1>"Not Started,TT in process,PVT/MC in process,Completed!!!"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J16" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J16">
       <formula1>"Not Started,Place &amp; Route in Process,DRC/LVS in Process,Completed!!!"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K2:K16" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" sqref="K2:K16">
       <formula1>"Not Started,Simulations in Progress,Completed!!!!"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F16" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F16">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A16 G2:G16 L2:L16" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B16" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A16 G2:G16 L2:L16"/>
+    <dataValidation type="list" allowBlank="1" sqref="B2:B16">
       <formula1>"P0,P1,P2,P3"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>